<commit_message>
Agregar archivo de Excel con códigos de barra para pedidos
</commit_message>
<xml_diff>
--- a/codigos_de_barra_pedidos.xlsx
+++ b/codigos_de_barra_pedidos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguil\Dev\Etiquetas_Amazon_Roberto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FE1196-416D-4E3E-8F11-D1CE541E4C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430D3C8A-A789-4619-9875-4EE95AE3D6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,28 +20,247 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
+  <si>
+    <t>FBAJV1003-BURDEOS42</t>
+  </si>
+  <si>
+    <t>FBAJV1003-CUERO42</t>
+  </si>
+  <si>
+    <t>FBAJV17001-MARRON40</t>
+  </si>
+  <si>
+    <t>FBAJV21300-BURDEOS38</t>
+  </si>
+  <si>
+    <t>FBAJV21300-NEGRO40</t>
+  </si>
+  <si>
+    <t>FBAJV3060-MARRON35</t>
+  </si>
+  <si>
+    <t>FBAJV3086-BEIGE38</t>
+  </si>
+  <si>
+    <t>FBAJV3086-BEIGE39</t>
+  </si>
+  <si>
+    <t>FBAJV3086-ROJO36</t>
+  </si>
+  <si>
+    <t>FBAJV3108-CUERO39</t>
+  </si>
+  <si>
+    <t>FBAJV3108-NEGRO40</t>
+  </si>
+  <si>
+    <t>FBAJV3108-ROJO39</t>
+  </si>
+  <si>
+    <t>FBAJV323-ROJO36</t>
+  </si>
+  <si>
+    <t>FBAJV323-ROJO38</t>
+  </si>
+  <si>
+    <t>FBAJV3454-ROJO36</t>
+  </si>
+  <si>
+    <t>FBAJV3454-ROJO38</t>
+  </si>
+  <si>
+    <t>FBAJV3454-ROJO41</t>
+  </si>
+  <si>
+    <t>FBAJV397-NEGRO41</t>
+  </si>
+  <si>
+    <t>FBAJV417-NEGRO39</t>
+  </si>
+  <si>
+    <t>FBAJV417-NEGRO41</t>
+  </si>
+  <si>
+    <t>FBAJV417-ROJO40</t>
+  </si>
+  <si>
+    <t>FBAJV6300-NEGRO41</t>
+  </si>
+  <si>
+    <t>FBAJV7740-BURDEOS37</t>
+  </si>
+  <si>
+    <t>FBAJV7740-BURDEOS38</t>
+  </si>
+  <si>
+    <t>FBAJV7740-BURDEOS39</t>
+  </si>
+  <si>
+    <t>FBAJV7740-NEGRO39</t>
+  </si>
+  <si>
+    <t>FBAJVAE220-CUERO41</t>
+  </si>
+  <si>
+    <t>FBAJVAE398-ROJO38</t>
+  </si>
+  <si>
+    <t>FBAJVAE398-ROJO39</t>
+  </si>
+  <si>
+    <t>FBAJVAE398-ROJO41</t>
+  </si>
+  <si>
+    <t>FBAJVCT441-NEGRO38</t>
+  </si>
+  <si>
+    <t>FBAJVCT441-NEGRO40</t>
+  </si>
+  <si>
+    <t>FBAJVFF4150-MARRON38</t>
+  </si>
+  <si>
+    <t>FBAJVFF4150-MARRON39</t>
+  </si>
+  <si>
+    <t>FBAJVFF4150-NEGRO38</t>
+  </si>
+  <si>
+    <t>FBAJVMX923-BURDEOS38</t>
+  </si>
+  <si>
+    <t>FBAJVMX923-BURDEOS40</t>
+  </si>
+  <si>
+    <t>FBAJVMX923-MARINO38</t>
+  </si>
+  <si>
+    <t>FBAJVMX923-NEGRO37</t>
+  </si>
+  <si>
+    <t>FBAJVMX923-NEGRO38</t>
+  </si>
+  <si>
+    <t>FBAJVMX923-NEGRO39</t>
+  </si>
+  <si>
+    <t>7427255118596</t>
+  </si>
+  <si>
+    <t>7427254911280</t>
+  </si>
+  <si>
+    <t>7427252422184</t>
+  </si>
+  <si>
+    <t>7427252424041</t>
+  </si>
+  <si>
+    <t>7427136757012</t>
+  </si>
+  <si>
+    <t>7427252421835</t>
+  </si>
+  <si>
+    <t>7427252421781</t>
+  </si>
+  <si>
+    <t>7427252421941</t>
+  </si>
+  <si>
+    <t>7427251888691</t>
+  </si>
+  <si>
+    <t>7427251481816</t>
+  </si>
+  <si>
+    <t>7427252427066</t>
+  </si>
+  <si>
+    <t>7427252423501</t>
+  </si>
+  <si>
+    <t>7427251889995</t>
+  </si>
+  <si>
+    <t>7427251890519</t>
+  </si>
+  <si>
+    <t>7427252426717</t>
+  </si>
+  <si>
+    <t>7427252426731</t>
+  </si>
+  <si>
+    <t>7427252426229</t>
+  </si>
+  <si>
+    <t>7427252426243</t>
+  </si>
+  <si>
+    <t>7427252426274</t>
+  </si>
+  <si>
+    <t>7427252423198</t>
+  </si>
+  <si>
+    <t>7427136792006</t>
+  </si>
+  <si>
+    <t>7427136792020</t>
+  </si>
+  <si>
+    <t>7427136792228</t>
+  </si>
+  <si>
+    <t>7427136791870</t>
+  </si>
+  <si>
+    <t>7427252424430</t>
+  </si>
+  <si>
+    <t>7427136751102</t>
+  </si>
+  <si>
+    <t>7427136751119</t>
+  </si>
+  <si>
+    <t>7427136751133</t>
+  </si>
+  <si>
+    <t>7427136792426</t>
+  </si>
+  <si>
+    <t>7427136792440</t>
+  </si>
+  <si>
+    <t>7427136751393</t>
+  </si>
+  <si>
+    <t>7427136751409</t>
+  </si>
+  <si>
+    <t>7427136751324</t>
+  </si>
   <si>
     <t>identificador_del_producto</t>
   </si>
   <si>
-    <t>FBAJV1003-NEGRO42</t>
-  </si>
-  <si>
-    <t>FBAJV1003-NEGRO44</t>
-  </si>
-  <si>
-    <t>FBAJV17001-MARRON35</t>
-  </si>
-  <si>
     <t>CODIGO DE BARRAS</t>
+  </si>
+  <si>
+    <t>FBAJAMTS553-IDAAZUL41</t>
+  </si>
+  <si>
+    <t>FBAJAMTS553-IDAAZUL40</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,10 +269,20 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF232F3E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -64,7 +293,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -87,34 +316,26 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -420,49 +641,426 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="28.42578125" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="8.85546875" style="3"/>
+    <col min="1" max="1" width="28.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B4" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4">
-        <v>7427252422115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="4">
-        <v>7427252422139</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="4">
-        <v>7427136756961</v>
+      <c r="B8" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="4">
+        <v>7427251219310</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="5">
+        <v>7427251219327</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="5">
+        <v>7427251219334</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="5">
+        <v>7427251219198</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="5">
+        <v>7427136756336</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="5">
+        <v>7427136756350</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="5">
+        <v>7427136756268</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="5">
+        <v>7427136756183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" s="5">
+        <v>7427136756190</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="5">
+        <v>7427136756190</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B50" s="5">
+        <v>7427136756206</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B51" s="5">
+        <v>7427136756206</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizar el archivo de Excel con códigos de barra para pedidos
</commit_message>
<xml_diff>
--- a/codigos_de_barra_pedidos.xlsx
+++ b/codigos_de_barra_pedidos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aguil\Dev\Etiquetas_Amazon_Roberto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430D3C8A-A789-4619-9875-4EE95AE3D6D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478FEDF8-C10A-4B5C-A460-CDEED18A0887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="89">
   <si>
     <t>FBAJV1003-BURDEOS42</t>
   </si>
@@ -254,6 +254,39 @@
   </si>
   <si>
     <t>FBAJAMTS553-IDAAZUL40</t>
+  </si>
+  <si>
+    <t>0742713675620</t>
+  </si>
+  <si>
+    <t>7427136756336</t>
+  </si>
+  <si>
+    <t>7427136756350</t>
+  </si>
+  <si>
+    <t>7427136756268</t>
+  </si>
+  <si>
+    <t>7427136756183</t>
+  </si>
+  <si>
+    <t>7427136756190</t>
+  </si>
+  <si>
+    <t>7427136756206</t>
+  </si>
+  <si>
+    <t>7427251219310</t>
+  </si>
+  <si>
+    <t>7427251219327</t>
+  </si>
+  <si>
+    <t>7427251219334</t>
+  </si>
+  <si>
+    <t>7427251219198</t>
   </si>
 </sst>
 </file>
@@ -325,16 +358,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -644,13 +677,13 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" style="4" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="2" customWidth="1"/>
     <col min="4" max="16384" width="8.85546875" style="2"/>
   </cols>
@@ -659,7 +692,7 @@
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>75</v>
       </c>
     </row>
@@ -667,7 +700,7 @@
       <c r="A2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -675,7 +708,7 @@
       <c r="A3" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>42</v>
       </c>
     </row>
@@ -683,7 +716,7 @@
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>43</v>
       </c>
     </row>
@@ -691,7 +724,7 @@
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>44</v>
       </c>
     </row>
@@ -699,7 +732,7 @@
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -707,7 +740,7 @@
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>46</v>
       </c>
     </row>
@@ -715,7 +748,7 @@
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -723,7 +756,7 @@
       <c r="A9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>47</v>
       </c>
     </row>
@@ -731,7 +764,7 @@
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -739,7 +772,7 @@
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>49</v>
       </c>
     </row>
@@ -747,7 +780,7 @@
       <c r="A12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>50</v>
       </c>
     </row>
@@ -755,7 +788,7 @@
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -763,7 +796,7 @@
       <c r="A14" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>52</v>
       </c>
     </row>
@@ -771,7 +804,7 @@
       <c r="A15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="4" t="s">
         <v>53</v>
       </c>
     </row>
@@ -779,7 +812,7 @@
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="4" t="s">
         <v>54</v>
       </c>
     </row>
@@ -787,7 +820,7 @@
       <c r="A17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="4" t="s">
         <v>55</v>
       </c>
     </row>
@@ -795,7 +828,7 @@
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -803,7 +836,7 @@
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="4" t="s">
         <v>57</v>
       </c>
     </row>
@@ -811,7 +844,7 @@
       <c r="A20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -819,7 +852,7 @@
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -883,39 +916,39 @@
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="4">
-        <v>7427251219310</v>
+      <c r="B29" s="4" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="5">
-        <v>7427251219327</v>
+      <c r="B30" s="5" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="5">
-        <v>7427251219334</v>
+      <c r="B31" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="5">
-        <v>7427251219198</v>
+      <c r="B32" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="4" t="s">
         <v>65</v>
       </c>
     </row>
@@ -923,7 +956,7 @@
       <c r="A34" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="4" t="s">
         <v>66</v>
       </c>
     </row>
@@ -931,7 +964,7 @@
       <c r="A35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="4" t="s">
         <v>66</v>
       </c>
     </row>
@@ -939,7 +972,7 @@
       <c r="A36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>67</v>
       </c>
     </row>
@@ -947,7 +980,7 @@
       <c r="A37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>68</v>
       </c>
     </row>
@@ -955,7 +988,7 @@
       <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>69</v>
       </c>
     </row>
@@ -963,7 +996,7 @@
       <c r="A39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="4" t="s">
         <v>70</v>
       </c>
     </row>
@@ -971,7 +1004,7 @@
       <c r="A40" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="4" t="s">
         <v>71</v>
       </c>
     </row>
@@ -979,7 +1012,7 @@
       <c r="A41" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="4" t="s">
         <v>72</v>
       </c>
     </row>
@@ -987,7 +1020,7 @@
       <c r="A42" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="4" t="s">
         <v>72</v>
       </c>
     </row>
@@ -995,7 +1028,7 @@
       <c r="A43" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1003,64 +1036,64 @@
       <c r="A44" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="5">
-        <v>7427136756336</v>
+      <c r="B44" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B45" s="5">
-        <v>7427136756350</v>
+      <c r="B45" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B46" s="5">
-        <v>7427136756268</v>
+      <c r="B46" s="5" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B47" s="5">
-        <v>7427136756183</v>
+      <c r="B47" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="5">
-        <v>7427136756190</v>
+      <c r="B48" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="5">
-        <v>7427136756190</v>
+      <c r="B49" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="5">
-        <v>7427136756206</v>
+      <c r="B50" s="5" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="5">
-        <v>7427136756206</v>
+      <c r="B51" s="5" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>